<commit_message>
Updated with birthdays and events.
</commit_message>
<xml_diff>
--- a/backend/calendar.xlsx
+++ b/backend/calendar.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="travel" sheetId="2" r:id="rId1"/>
     <sheet name="training" sheetId="1" r:id="rId2"/>
+    <sheet name="events" sheetId="3" r:id="rId3"/>
+    <sheet name="birthdays" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="owssvr__28" localSheetId="1" hidden="1">training!$A$1:$H$28</definedName>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="123">
   <si>
     <t>Title</t>
   </si>
@@ -375,12 +377,39 @@
   </si>
   <si>
     <t>Thomas Gustafsson and Tomas Damgaard</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Anusha</t>
+  </si>
+  <si>
+    <t>Prashanth</t>
+  </si>
+  <si>
+    <t>Swaroop</t>
+  </si>
+  <si>
+    <t>Vignesh</t>
+  </si>
+  <si>
+    <t>Manu Mohey</t>
+  </si>
+  <si>
+    <t>Karthik NS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+  </numFmts>
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -517,7 +546,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -697,8 +726,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -813,6 +854,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -858,11 +936,28 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -921,10 +1016,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -946,10 +1041,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1010,13 +1105,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_owssvr__29" displayName="Table_owssvr__29" ref="A1:H75" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" uniqueName="fRecurrence" name="Recurrence" queryTableFieldId="6"/>
-    <tableColumn id="2" uniqueName="Title" name="Title" queryTableFieldId="1" dataDxfId="6"/>
-    <tableColumn id="3" uniqueName="Location" name="Location" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="4" uniqueName="EventDate" name="Start Time" queryTableFieldId="3" dataDxfId="4"/>
-    <tableColumn id="5" uniqueName="EndDate" name="End Time" queryTableFieldId="4" dataDxfId="3"/>
-    <tableColumn id="6" uniqueName="fAllDayEvent" name="All Day Event" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="7" uniqueName="FSObjType" name="Item Type" queryTableFieldId="8" dataDxfId="1"/>
-    <tableColumn id="8" uniqueName="FileDirRef" name="Path" queryTableFieldId="7" dataDxfId="0"/>
+    <tableColumn id="2" uniqueName="Title" name="Title" queryTableFieldId="1" dataDxfId="13"/>
+    <tableColumn id="3" uniqueName="Location" name="Location" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="4" uniqueName="EventDate" name="Start Time" queryTableFieldId="3" dataDxfId="11"/>
+    <tableColumn id="5" uniqueName="EndDate" name="End Time" queryTableFieldId="4" dataDxfId="10"/>
+    <tableColumn id="6" uniqueName="fAllDayEvent" name="All Day Event" queryTableFieldId="5" dataDxfId="9"/>
+    <tableColumn id="7" uniqueName="FSObjType" name="Item Type" queryTableFieldId="8" dataDxfId="8"/>
+    <tableColumn id="8" uniqueName="FileDirRef" name="Path" queryTableFieldId="7" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1026,13 +1121,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr__28" displayName="Table_owssvr__28" ref="A1:H28" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" uniqueName="fRecurrence" name="Recurrence" queryTableFieldId="8"/>
-    <tableColumn id="2" uniqueName="Title" name="Title" queryTableFieldId="1" dataDxfId="13"/>
-    <tableColumn id="3" uniqueName="Location" name="Location" queryTableFieldId="4" dataDxfId="12"/>
-    <tableColumn id="4" uniqueName="EventDate" name="Start Time" queryTableFieldId="5" dataDxfId="11"/>
-    <tableColumn id="5" uniqueName="EndDate" name="End Time" queryTableFieldId="6" dataDxfId="10"/>
-    <tableColumn id="6" uniqueName="fAllDayEvent" name="All Day Event" queryTableFieldId="7" dataDxfId="9"/>
-    <tableColumn id="7" uniqueName="FSObjType" name="Item Type" queryTableFieldId="3" dataDxfId="8"/>
-    <tableColumn id="8" uniqueName="FileDirRef" name="Path" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="2" uniqueName="Title" name="Title" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="3" uniqueName="Location" name="Location" queryTableFieldId="4" dataDxfId="5"/>
+    <tableColumn id="4" uniqueName="EventDate" name="Start Time" queryTableFieldId="5" dataDxfId="4"/>
+    <tableColumn id="5" uniqueName="EndDate" name="End Time" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="6" uniqueName="fAllDayEvent" name="All Day Event" queryTableFieldId="7" dataDxfId="2"/>
+    <tableColumn id="7" uniqueName="FSObjType" name="Item Type" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="8" uniqueName="FileDirRef" name="Path" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1293,7 +1388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1303,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3137,7 +3232,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection sqref="A1:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3867,4 +3962,570 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="9">
+        <v>43104</v>
+      </c>
+      <c r="E2" s="9">
+        <v>43105.999305555553</v>
+      </c>
+      <c r="F2" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14">
+        <v>43115</v>
+      </c>
+      <c r="E3" s="14">
+        <v>43119.999305555553</v>
+      </c>
+      <c r="F3" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="9">
+        <v>43115</v>
+      </c>
+      <c r="E4" s="9">
+        <v>43119.999305555553</v>
+      </c>
+      <c r="F4" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="14">
+        <v>43123.395833333336</v>
+      </c>
+      <c r="E5" s="14">
+        <v>43123.520833333336</v>
+      </c>
+      <c r="F5" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9">
+        <v>43133</v>
+      </c>
+      <c r="E6" s="9">
+        <v>43133.999305555553</v>
+      </c>
+      <c r="F6" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14">
+        <v>43136.5</v>
+      </c>
+      <c r="E7" s="14">
+        <v>43137.541666666664</v>
+      </c>
+      <c r="F7" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9">
+        <v>43144</v>
+      </c>
+      <c r="E8" s="9">
+        <v>43147.999305555553</v>
+      </c>
+      <c r="F8" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14">
+        <v>43150</v>
+      </c>
+      <c r="E9" s="14">
+        <v>43151.999305555553</v>
+      </c>
+      <c r="F9" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9">
+        <v>43168.583333333336</v>
+      </c>
+      <c r="E10" s="9">
+        <v>43168.666666666664</v>
+      </c>
+      <c r="F10" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14">
+        <v>43185</v>
+      </c>
+      <c r="E11" s="14">
+        <v>43188.999305555553</v>
+      </c>
+      <c r="F11" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="9">
+        <v>43206</v>
+      </c>
+      <c r="E12" s="9">
+        <v>43208.999305555553</v>
+      </c>
+      <c r="F12" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14">
+        <v>43235.458333333336</v>
+      </c>
+      <c r="E13" s="14">
+        <v>43235.5</v>
+      </c>
+      <c r="F13" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="9">
+        <v>43238.416666666664</v>
+      </c>
+      <c r="E14" s="9">
+        <v>43238.541666666664</v>
+      </c>
+      <c r="F14" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="14">
+        <v>43255.375</v>
+      </c>
+      <c r="E15" s="14">
+        <v>43259.791666666664</v>
+      </c>
+      <c r="F15" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="9">
+        <v>43294.4375</v>
+      </c>
+      <c r="E16" s="9">
+        <v>43294.541666666664</v>
+      </c>
+      <c r="F16" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="14">
+        <v>43301.416666666664</v>
+      </c>
+      <c r="E17" s="14">
+        <v>43301.541666666664</v>
+      </c>
+      <c r="F17" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="19">
+        <v>17394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="20">
+        <v>31679</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="19">
+        <v>36872</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="20">
+        <v>34188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="19">
+        <v>41129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="20">
+        <v>43136.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="18"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="13"/>
+      <c r="B11" s="18"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="13"/>
+      <c r="B13" s="18"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="13"/>
+      <c r="B15" s="18"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added scss files to build custom css for bulma and the calendar.
</commit_message>
<xml_diff>
--- a/backend/calendar.xlsx
+++ b/backend/calendar.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\blrroot\project\Shared_VAI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11700" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="travel" sheetId="2" r:id="rId1"/>
     <sheet name="training" sheetId="1" r:id="rId2"/>
-    <sheet name="events" sheetId="3" r:id="rId3"/>
-    <sheet name="birthdays" sheetId="4" r:id="rId4"/>
+    <sheet name="events" sheetId="5" r:id="rId3"/>
+    <sheet name="birthdays" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="owssvr__28" localSheetId="1" hidden="1">training!$A$1:$H$28</definedName>
-    <definedName name="owssvr__29" localSheetId="0" hidden="1">travel!$A$1:$H$75</definedName>
+    <definedName name="owssvr__28" localSheetId="1" hidden="1">training!$A$1:$H$29</definedName>
+    <definedName name="owssvr__29" localSheetId="0" hidden="1">travel!$A$1:$H$93</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="145">
   <si>
     <t>Title</t>
   </si>
@@ -379,38 +384,101 @@
     <t>Thomas Gustafsson and Tomas Damgaard</t>
   </si>
   <si>
+    <t>Info session - AES Geometric Data Migration and MBD</t>
+  </si>
+  <si>
+    <t>Arun Kumar Swaminathan's travel to US</t>
+  </si>
+  <si>
+    <t>Ravikumar Karpuram's travel to UK</t>
+  </si>
+  <si>
+    <t>Prarthana and Cedric's travel to UK</t>
+  </si>
+  <si>
+    <t>Prarthana's return from UK</t>
+  </si>
+  <si>
+    <t>Ravikumar Karpuram's return from UK</t>
+  </si>
+  <si>
+    <t>Cedric's return from UK</t>
+  </si>
+  <si>
+    <t>Prarthana's travel to Netherlands</t>
+  </si>
+  <si>
+    <t>Prarthana's return from Netherlands</t>
+  </si>
+  <si>
+    <t>Kumaran's travel to the US</t>
+  </si>
+  <si>
+    <t>Ian Bamforth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark Shufflebotham and Martin Robinson </t>
+  </si>
+  <si>
+    <t>Ulrich Scheibe</t>
+  </si>
+  <si>
+    <t>Thulasi's travel to Sweden</t>
+  </si>
+  <si>
+    <t>Thulasi's return from Sweden</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
     <t>Date of Birth</t>
   </si>
   <si>
-    <t>Anusha</t>
-  </si>
-  <si>
-    <t>Prashanth</t>
-  </si>
-  <si>
-    <t>Swaroop</t>
-  </si>
-  <si>
-    <t>Vignesh</t>
-  </si>
-  <si>
-    <t>Manu Mohey</t>
-  </si>
-  <si>
-    <t>Karthik NS</t>
+    <t>Pawan C Ganapathy</t>
+  </si>
+  <si>
+    <t>Vignesh B</t>
+  </si>
+  <si>
+    <t>Alden  Cornelio</t>
+  </si>
+  <si>
+    <t>Sravan  Shakker</t>
+  </si>
+  <si>
+    <t>Siddarth  Aghanashini</t>
+  </si>
+  <si>
+    <t>Latha R</t>
+  </si>
+  <si>
+    <t>Thulasi  Ramachandran</t>
+  </si>
+  <si>
+    <t>Dhirendra Singh Chauhan</t>
+  </si>
+  <si>
+    <t>Pradeep Pothuganti</t>
+  </si>
+  <si>
+    <t>Jeevanandham's travel to UK</t>
+  </si>
+  <si>
+    <t>Jeevanandham's return from UK</t>
+  </si>
+  <si>
+    <t>Satish's travel to Hong Kong</t>
+  </si>
+  <si>
+    <t>Satish's return from Hong Kong</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-  </numFmts>
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,6 +609,17 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -728,18 +807,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -891,6 +970,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -936,28 +1030,43 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="22" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1016,10 +1125,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1041,10 +1150,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1102,7 +1211,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_owssvr__29" displayName="Table_owssvr__29" ref="A1:H75" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_owssvr__29" displayName="Table_owssvr__29" ref="A1:H93" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" uniqueName="fRecurrence" name="Recurrence" queryTableFieldId="6"/>
     <tableColumn id="2" uniqueName="Title" name="Title" queryTableFieldId="1" dataDxfId="13"/>
@@ -1118,7 +1227,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr__28" displayName="Table_owssvr__28" ref="A1:H28" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr__28" displayName="Table_owssvr__28" ref="A1:H29" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
     <tableColumn id="1" uniqueName="fRecurrence" name="Recurrence" queryTableFieldId="8"/>
     <tableColumn id="2" uniqueName="Title" name="Title" queryTableFieldId="1" dataDxfId="6"/>
@@ -1388,7 +1497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1396,24 +1505,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1439,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>0</v>
       </c>
@@ -1463,7 +1572,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -1487,7 +1596,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -1511,7 +1620,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -1535,7 +1644,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="b">
         <v>0</v>
       </c>
@@ -1559,7 +1668,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -1583,7 +1692,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -1607,7 +1716,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="b">
         <v>0</v>
       </c>
@@ -1631,7 +1740,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -1655,7 +1764,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -1679,7 +1788,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -1703,7 +1812,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="b">
         <v>0</v>
       </c>
@@ -1727,7 +1836,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="b">
         <v>0</v>
       </c>
@@ -1751,7 +1860,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -1775,7 +1884,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -1799,7 +1908,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -1823,7 +1932,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -1847,7 +1956,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -1871,7 +1980,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -1895,7 +2004,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -1919,7 +2028,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -1943,7 +2052,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -1967,7 +2076,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -1993,7 +2102,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -2017,7 +2126,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -2041,7 +2150,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -2065,7 +2174,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -2089,7 +2198,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="b">
         <v>0</v>
       </c>
@@ -2113,7 +2222,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="b">
         <v>0</v>
       </c>
@@ -2137,7 +2246,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="b">
         <v>0</v>
       </c>
@@ -2161,7 +2270,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="b">
         <v>0</v>
       </c>
@@ -2185,7 +2294,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="b">
         <v>0</v>
       </c>
@@ -2209,7 +2318,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="b">
         <v>0</v>
       </c>
@@ -2233,7 +2342,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="b">
         <v>0</v>
       </c>
@@ -2257,7 +2366,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="b">
         <v>0</v>
       </c>
@@ -2281,7 +2390,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="b">
         <v>0</v>
       </c>
@@ -2305,7 +2414,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="b">
         <v>0</v>
       </c>
@@ -2329,7 +2438,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="b">
         <v>0</v>
       </c>
@@ -2353,7 +2462,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="b">
         <v>0</v>
       </c>
@@ -2377,7 +2486,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="b">
         <v>0</v>
       </c>
@@ -2401,7 +2510,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="b">
         <v>0</v>
       </c>
@@ -2425,7 +2534,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="b">
         <v>0</v>
       </c>
@@ -2449,7 +2558,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="b">
         <v>0</v>
       </c>
@@ -2473,7 +2582,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="b">
         <v>0</v>
       </c>
@@ -2497,7 +2606,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="b">
         <v>0</v>
       </c>
@@ -2521,7 +2630,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="b">
         <v>0</v>
       </c>
@@ -2545,7 +2654,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="b">
         <v>0</v>
       </c>
@@ -2569,7 +2678,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="b">
         <v>0</v>
       </c>
@@ -2593,7 +2702,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="b">
         <v>0</v>
       </c>
@@ -2617,7 +2726,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="b">
         <v>0</v>
       </c>
@@ -2641,7 +2750,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="b">
         <v>0</v>
       </c>
@@ -2665,7 +2774,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="b">
         <v>0</v>
       </c>
@@ -2689,7 +2798,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="b">
         <v>0</v>
       </c>
@@ -2713,7 +2822,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="b">
         <v>0</v>
       </c>
@@ -2737,7 +2846,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="b">
         <v>0</v>
       </c>
@@ -2761,7 +2870,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="b">
         <v>0</v>
       </c>
@@ -2785,7 +2894,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="b">
         <v>0</v>
       </c>
@@ -2809,7 +2918,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="b">
         <v>0</v>
       </c>
@@ -2833,7 +2942,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="b">
         <v>0</v>
       </c>
@@ -2857,7 +2966,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="b">
         <v>0</v>
       </c>
@@ -2881,7 +2990,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="b">
         <v>0</v>
       </c>
@@ -2905,7 +3014,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="b">
         <v>0</v>
       </c>
@@ -2929,7 +3038,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="b">
         <v>0</v>
       </c>
@@ -2953,7 +3062,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="b">
         <v>0</v>
       </c>
@@ -2977,7 +3086,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="b">
         <v>0</v>
       </c>
@@ -3001,7 +3110,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="b">
         <v>0</v>
       </c>
@@ -3025,7 +3134,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="b">
         <v>0</v>
       </c>
@@ -3049,7 +3158,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="b">
         <v>0</v>
       </c>
@@ -3073,7 +3182,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="b">
         <v>0</v>
       </c>
@@ -3097,7 +3206,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="b">
         <v>0</v>
       </c>
@@ -3123,19 +3232,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="b">
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="2">
-        <v>43310</v>
+        <v>43294</v>
       </c>
       <c r="E72" s="2">
-        <v>43310.999305555553</v>
+        <v>43294.999305555553</v>
       </c>
       <c r="F72" s="3" t="b">
         <v>1</v>
@@ -3147,19 +3256,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="b">
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="2">
-        <v>43318</v>
+        <v>43296</v>
       </c>
       <c r="E73" s="2">
-        <v>43318.999305555553</v>
+        <v>43296.999305555553</v>
       </c>
       <c r="F73" s="3" t="b">
         <v>1</v>
@@ -3171,19 +3280,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="b">
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="2">
-        <v>43344</v>
+        <v>43297</v>
       </c>
       <c r="E74" s="2">
-        <v>43344.999305555553</v>
+        <v>43297.999305555553</v>
       </c>
       <c r="F74" s="3" t="b">
         <v>1</v>
@@ -3195,58 +3304,491 @@
         <v>42</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="b">
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="2">
+        <v>43301</v>
+      </c>
+      <c r="E75" s="2">
+        <v>43301.999305555553</v>
+      </c>
+      <c r="F75" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="b">
+        <v>0</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="2">
+        <v>43303</v>
+      </c>
+      <c r="E76" s="2">
+        <v>43303.999305555553</v>
+      </c>
+      <c r="F76" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="b">
+        <v>0</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="2">
+        <v>43303</v>
+      </c>
+      <c r="E77" s="2">
+        <v>43303.999305555553</v>
+      </c>
+      <c r="F77" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="b">
+        <v>0</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="2">
+        <v>43310</v>
+      </c>
+      <c r="E78" s="2">
+        <v>43310.999305555553</v>
+      </c>
+      <c r="F78" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="b">
+        <v>0</v>
+      </c>
+      <c r="B79" t="s">
+        <v>125</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="2">
+        <v>43316</v>
+      </c>
+      <c r="E79" s="2">
+        <v>43319</v>
+      </c>
+      <c r="F79" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="b">
+        <v>0</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="D80" s="2">
+        <v>43316</v>
+      </c>
+      <c r="E80" s="2">
+        <v>43325</v>
+      </c>
+      <c r="F80" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="b">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C81" s="1"/>
+      <c r="D81" s="2">
+        <v>43318</v>
+      </c>
+      <c r="E81" s="2">
+        <v>43318.999305555553</v>
+      </c>
+      <c r="F81" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="b">
+        <v>0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="2">
+        <v>43321</v>
+      </c>
+      <c r="E82" s="2">
+        <v>43321.999305555553</v>
+      </c>
+      <c r="F82" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="b">
+        <v>0</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="2">
+        <v>43331</v>
+      </c>
+      <c r="E83" s="2">
+        <v>43331.999305555553</v>
+      </c>
+      <c r="F83" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="b">
+        <v>0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="D84" s="2">
+        <v>43338</v>
+      </c>
+      <c r="E84" s="2">
+        <v>43338.999305555553</v>
+      </c>
+      <c r="F84" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="b">
+        <v>0</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C85" s="1"/>
+      <c r="D85" s="2">
+        <v>43344</v>
+      </c>
+      <c r="E85" s="2">
+        <v>43344.999305555553</v>
+      </c>
+      <c r="F85" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="b">
+        <v>0</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="D86" s="2">
         <v>43348</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E86" s="2">
         <v>43350.999305555553</v>
       </c>
-      <c r="F75" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H75" s="1" t="s">
+      <c r="F86" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="b">
+        <v>0</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C87" s="1"/>
+      <c r="D87" s="2">
+        <v>43347</v>
+      </c>
+      <c r="E87" s="2">
+        <v>43350.999305555553</v>
+      </c>
+      <c r="F87" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="b">
+        <v>0</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C88" s="1"/>
+      <c r="D88" s="2">
+        <v>43346</v>
+      </c>
+      <c r="E88" s="2">
+        <v>43346</v>
+      </c>
+      <c r="F88" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="b">
+        <v>0</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="2">
+        <v>43413</v>
+      </c>
+      <c r="E89" s="2">
+        <v>43413</v>
+      </c>
+      <c r="F89" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="b">
+        <v>0</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C90" s="1"/>
+      <c r="D90" s="2">
+        <v>43351</v>
+      </c>
+      <c r="E90" s="2">
+        <v>43351</v>
+      </c>
+      <c r="F90" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="b">
+        <v>0</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="2">
+        <v>43359</v>
+      </c>
+      <c r="E91" s="2">
+        <v>43359</v>
+      </c>
+      <c r="F91" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="b">
+        <v>0</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="2">
+        <v>43354</v>
+      </c>
+      <c r="E92" s="2">
+        <v>43354</v>
+      </c>
+      <c r="F92" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" t="b">
+        <v>0</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C93" s="1"/>
+      <c r="D93" s="2">
+        <v>43356</v>
+      </c>
+      <c r="E93" s="2">
+        <v>43356</v>
+      </c>
+      <c r="F93" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H93" s="1" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H17"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -3272,7 +3814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>0</v>
       </c>
@@ -3298,7 +3840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -3322,7 +3864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -3348,7 +3890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -3374,7 +3916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="b">
         <v>0</v>
       </c>
@@ -3398,7 +3940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -3422,7 +3964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -3446,7 +3988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="b">
         <v>0</v>
       </c>
@@ -3470,7 +4012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -3494,7 +4036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -3518,7 +4060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -3544,7 +4086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="b">
         <v>0</v>
       </c>
@@ -3568,7 +4110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="b">
         <v>0</v>
       </c>
@@ -3594,7 +4136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="b">
         <v>1</v>
       </c>
@@ -3620,7 +4162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -3646,21 +4188,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="b">
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="2">
-        <v>43301.416666666664</v>
+        <v>43300.458333333336</v>
       </c>
       <c r="E17" s="2">
-        <v>43301.541666666664</v>
+        <v>43300.5</v>
       </c>
       <c r="F17" s="3" t="b">
         <v>0</v>
@@ -3672,24 +4214,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="b">
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="2">
-        <v>43305</v>
+        <v>43301.416666666664</v>
       </c>
       <c r="E18" s="2">
-        <v>43306.999305555553</v>
+        <v>43301.541666666664</v>
       </c>
       <c r="F18" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>10</v>
@@ -3698,22 +4240,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="b">
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D19" s="2">
-        <v>43308.4375</v>
+        <v>43305</v>
       </c>
       <c r="E19" s="2">
-        <v>43308.5</v>
+        <v>43306.999305555553</v>
       </c>
       <c r="F19" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>10</v>
@@ -3722,21 +4266,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="b">
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="2">
-        <v>43314.375</v>
+        <v>43308.4375</v>
       </c>
       <c r="E20" s="2">
-        <v>43314.75</v>
+        <v>43308.5</v>
       </c>
       <c r="F20" s="3" t="b">
         <v>0</v>
@@ -3748,21 +4290,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="b">
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="2">
-        <v>43320.416666666664</v>
+        <v>43314.375</v>
       </c>
       <c r="E21" s="2">
-        <v>43320.5</v>
+        <v>43314.75</v>
       </c>
       <c r="F21" s="3" t="b">
         <v>0</v>
@@ -3774,7 +4316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -3800,7 +4342,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -3826,21 +4368,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="b">
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="2">
-        <v>43349.416666666664</v>
+        <v>43357.375</v>
       </c>
       <c r="E24" s="2">
-        <v>43349.5</v>
+        <v>43357.541666666664</v>
       </c>
       <c r="F24" s="3" t="b">
         <v>0</v>
@@ -3852,24 +4394,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="b">
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="2">
-        <v>43357.375</v>
+        <v>43364</v>
       </c>
       <c r="E25" s="2">
-        <v>43357.541666666664</v>
+        <v>43364.999305555553</v>
       </c>
       <c r="F25" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>10</v>
@@ -3878,24 +4420,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="b">
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="2">
-        <v>43364</v>
+        <v>43371.416666666664</v>
       </c>
       <c r="E26" s="2">
-        <v>43364.999305555553</v>
+        <v>43371.5</v>
       </c>
       <c r="F26" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>10</v>
@@ -3904,7 +4446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -3930,29 +4472,55 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="b">
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D28" s="2">
+        <v>43392.416666666664</v>
+      </c>
+      <c r="E28" s="2">
+        <v>43392.5</v>
+      </c>
+      <c r="F28" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="2">
         <v>43399.416666666664</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E29" s="2">
         <v>43399.5</v>
       </c>
-      <c r="F28" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="1" t="s">
+      <c r="F29" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3969,443 +4537,443 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="H1" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="11">
         <v>43104</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="11">
         <v>43105.999305555553</v>
       </c>
-      <c r="F2" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="11" t="s">
+      <c r="F2" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14">
+      <c r="C3" s="5"/>
+      <c r="D3" s="6">
         <v>43115</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="6">
         <v>43119.999305555553</v>
       </c>
-      <c r="F3" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="16" t="s">
+      <c r="F3" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="11">
         <v>43115</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="11">
         <v>43119.999305555553</v>
       </c>
-      <c r="F4" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="11" t="s">
+      <c r="F4" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="6">
         <v>43123.395833333336</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="6">
         <v>43123.520833333336</v>
       </c>
-      <c r="F5" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="16" t="s">
+      <c r="F5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9">
+      <c r="C6" s="10"/>
+      <c r="D6" s="11">
         <v>43133</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="11">
         <v>43133.999305555553</v>
       </c>
-      <c r="F6" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="11" t="s">
+      <c r="F6" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B7" s="13" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14">
+      <c r="C7" s="5"/>
+      <c r="D7" s="6">
         <v>43136.5</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="6">
         <v>43137.541666666664</v>
       </c>
-      <c r="F7" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="16" t="s">
+      <c r="F7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9">
+      <c r="C8" s="10"/>
+      <c r="D8" s="11">
         <v>43144</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="11">
         <v>43147.999305555553</v>
       </c>
-      <c r="F8" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="11" t="s">
+      <c r="F8" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14">
+      <c r="C9" s="5"/>
+      <c r="D9" s="6">
         <v>43150</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="6">
         <v>43151.999305555553</v>
       </c>
-      <c r="F9" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="16" t="s">
+      <c r="F9" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9">
+      <c r="C10" s="10"/>
+      <c r="D10" s="11">
         <v>43168.583333333336</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="11">
         <v>43168.666666666664</v>
       </c>
-      <c r="F10" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="11" t="s">
+      <c r="F10" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B11" s="13" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14">
+      <c r="C11" s="5"/>
+      <c r="D11" s="6">
         <v>43185</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="6">
         <v>43188.999305555553</v>
       </c>
-      <c r="F11" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="16" t="s">
+      <c r="F11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="B12" s="8" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="11">
         <v>43206</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="11">
         <v>43208.999305555553</v>
       </c>
-      <c r="F12" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="11" t="s">
+      <c r="F12" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B13" s="13" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14">
+      <c r="C13" s="5"/>
+      <c r="D13" s="6">
         <v>43235.458333333336</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="6">
         <v>43235.5</v>
       </c>
-      <c r="F13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="16" t="s">
+      <c r="F13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="B14" s="8" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="11">
         <v>43238.416666666664</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="11">
         <v>43238.541666666664</v>
       </c>
-      <c r="F14" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="11" t="s">
+      <c r="F14" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="B15" s="13" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="6">
         <v>43255.375</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="6">
         <v>43259.791666666664</v>
       </c>
-      <c r="F15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="16" t="s">
+      <c r="F15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="11">
         <v>43294.4375</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="11">
         <v>43294.541666666664</v>
       </c>
-      <c r="F16" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="11" t="s">
+      <c r="F16" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="6">
         <v>43301.416666666664</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="6">
         <v>43301.541666666664</v>
       </c>
-      <c r="F17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="16" t="s">
+      <c r="F17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4416,113 +4984,101 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="8" t="s">
-        <v>117</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>132</v>
       </c>
       <c r="B2" s="19">
-        <v>17394</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="20">
-        <v>31679</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="19">
-        <v>36872</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="20">
-        <v>34188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="8" t="s">
-        <v>121</v>
+        <v>42949</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="21">
+        <v>42954</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="23">
+        <v>42965</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="19">
+        <v>42969</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>135</v>
       </c>
       <c r="B6" s="19">
-        <v>41129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="20">
-        <v>43136.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="17"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="18"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="17"/>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="18"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="17"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="18"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="17"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="18"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="17"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="18"/>
+        <v>42969</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="22">
+        <v>42972</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="22">
+        <v>43338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="19">
+        <v>42976</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="19">
+        <v>42977</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>